<commit_message>
updating complexity conversions, adding experimental condition plots
</commit_message>
<xml_diff>
--- a/detectors.xlsx
+++ b/detectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390DFE04-F250-0448-B354-A529D905281B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F530F8-88C7-0442-9B9D-80F53CAB7DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2700" windowWidth="25420" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15020" yWindow="2200" windowWidth="36180" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="7" r:id="rId1"/>
@@ -875,36 +875,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Detector Data</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Rate vs. Year</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -943,6 +913,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Instantaneous Luminosity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -965,98 +946,12 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>summary!$A$2:$A$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1982</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1989</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1989</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1992</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1992</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2025</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>summary!$F$2:$F$17</c:f>
+              <c:f>summary!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>8000000000</c:v>
                 </c:pt>
@@ -1092,11 +987,53 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>summary!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.9999999999999999E+31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999996E+30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999996E+30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6E+31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6E+31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0000000000000002E+32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0000000000000002E+32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E+33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9999999999999995E+33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7E+34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7E+34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DFD1-384F-8946-3D3CF2F422F9}"/>
+              <c16:uniqueId val="{00000000-150F-AB44-8756-94CFD9CCE26F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1108,12 +1045,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="454910879"/>
-        <c:axId val="522599743"/>
+        <c:axId val="2014740144"/>
+        <c:axId val="2028158736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="454910879"/>
+        <c:axId val="2014740144"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1132,7 +1070,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1169,16 +1107,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522599743"/>
+        <c:crossAx val="2028158736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="522599743"/>
+        <c:axId val="2028158736"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="1000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1233,7 +1169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454910879"/>
+        <c:crossAx val="2014740144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1290,6 +1226,422 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Instantaneous Luminosity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9474628171478565E-2"/>
+                  <c:y val="0.14310185185185181"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>summary!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.9999999999999999E+31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999996E+30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999996E+30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6E+31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6E+31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0000000000000002E+32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0000000000000002E+32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E+33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9999999999999995E+33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7E+34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7E+34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>summary!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8000000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>585000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1350000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1041666666666.6666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1041666666666.6666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77142857142.857147</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85714285714.285721</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000000000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64000000000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>320000000000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>176000000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8B7A-F74B-94C8-F74AAECDF247}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="926030768"/>
+        <c:axId val="926033040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="926030768"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="926033040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="926033040"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="926030768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1661,7 +2013,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2112,6 +2464,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3145,6 +3537,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3665,22 +4573,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>644072</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>39009</xdr:rowOff>
+      <xdr:colOff>77108</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>108857</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>187780</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00371A5B-469D-6C0B-33DA-56714A1898AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C397B44-2547-7DA7-2C86-A0089989ADDF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3693,6 +4601,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>789214</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>408214</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D76BB53-CD71-DAE7-F26E-8BCF52163341}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4078,7 +5022,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>